<commit_message>
added games for March and April 2024 to SQL database and all files
</commit_message>
<xml_diff>
--- a/games_collections/playstation/SQL Output/Complete Database/complete_info.xlsx
+++ b/games_collections/playstation/SQL Output/Complete Database/complete_info.xlsx
@@ -3,22 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="2024-03-24" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2024-04-04" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'2024-03-24'!$A$1:$I$938</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'2024-04-04'!$A$1:$I$942</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="PEthyJPNY6IbQmPySyaF99oadExI2vahq4iNgEqXm3k="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Ghv/EAdbn7XBhOq3dySBHO0ElfCWoHgHQA2NDf/rO1c="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3758" uniqueCount="1516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="1522">
   <si>
     <t>ID</t>
   </si>
@@ -4566,6 +4566,24 @@
   </si>
   <si>
     <t>Goat Simulator 3</t>
+  </si>
+  <si>
+    <t>EA Sports FC 24</t>
+  </si>
+  <si>
+    <t>The Survivalists: Deluxe Edition</t>
+  </si>
+  <si>
+    <t>Minecraft Legends</t>
+  </si>
+  <si>
+    <t>Skul: The Hero Slayer</t>
+  </si>
+  <si>
+    <t>SouthPAW Games</t>
+  </si>
+  <si>
+    <t>AVG per Year (across 16 Years)</t>
   </si>
 </sst>
 </file>
@@ -4576,7 +4594,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="[$€]#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -4597,6 +4615,10 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -4631,7 +4653,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4653,16 +4675,28 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -32098,58 +32132,196 @@
         <v>56</v>
       </c>
     </row>
+    <row r="939">
+      <c r="A939" s="7">
+        <v>938.0</v>
+      </c>
+      <c r="B939" s="7" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C939" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D939" s="8">
+        <v>45377.0</v>
+      </c>
+      <c r="E939" s="9">
+        <v>79.99</v>
+      </c>
+      <c r="F939" s="9">
+        <v>15.99</v>
+      </c>
+      <c r="G939" s="9">
+        <f t="shared" ref="G939:G942" si="1">E939-F939</f>
+        <v>64</v>
+      </c>
+      <c r="H939" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I939" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="940">
-      <c r="E940" s="7">
-        <f t="shared" ref="E940:G940" si="1">SUM(E2:E938)</f>
-        <v>22630.22</v>
-      </c>
-      <c r="F940" s="7">
+      <c r="A940" s="7">
+        <v>939.0</v>
+      </c>
+      <c r="B940" s="7" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C940" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D940" s="8">
+        <v>45382.0</v>
+      </c>
+      <c r="E940" s="9">
+        <v>26.48</v>
+      </c>
+      <c r="F940" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G940" s="9">
         <f t="shared" si="1"/>
-        <v>10180.7</v>
-      </c>
-      <c r="G940" s="7">
+        <v>26.48</v>
+      </c>
+      <c r="H940" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I940" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" s="7">
+        <v>940.0</v>
+      </c>
+      <c r="B941" s="7" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C941" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D941" s="8">
+        <v>45385.0</v>
+      </c>
+      <c r="E941" s="9">
+        <v>39.99</v>
+      </c>
+      <c r="F941" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G941" s="9">
         <f t="shared" si="1"/>
-        <v>12449.52</v>
-      </c>
-      <c r="H940" s="8">
-        <f t="shared" ref="H940:H941" si="2">E940-F940</f>
-        <v>12449.52</v>
-      </c>
-      <c r="I940" s="9">
-        <f>COUNTA(I2:I939)</f>
-        <v>937</v>
-      </c>
-    </row>
-    <row r="941">
-      <c r="E941" s="7">
-        <f>E940/I940</f>
-        <v>24.15178228</v>
-      </c>
-      <c r="F941" s="7">
-        <f>F940/I940</f>
-        <v>10.86520811</v>
-      </c>
-      <c r="G941" s="7">
-        <f>G940/I940</f>
-        <v>13.28657417</v>
-      </c>
-      <c r="H941" s="8">
+        <v>39.99</v>
+      </c>
+      <c r="H941" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="I941" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="7">
+        <v>941.0</v>
+      </c>
+      <c r="B942" s="7" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C942" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D942" s="8">
+        <v>45385.0</v>
+      </c>
+      <c r="E942" s="9">
+        <v>16.99</v>
+      </c>
+      <c r="F942" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G942" s="9">
+        <f t="shared" si="1"/>
+        <v>16.99</v>
+      </c>
+      <c r="H942" s="2" t="s">
+        <v>1520</v>
+      </c>
+      <c r="I942" s="2" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="E944" s="10">
+        <f t="shared" ref="E944:G944" si="2">SUM(E2:E942)</f>
+        <v>22793.67</v>
+      </c>
+      <c r="F944" s="10">
         <f t="shared" si="2"/>
-        <v>13.28657417</v>
-      </c>
-      <c r="I941" s="9">
-        <f>I940/I940</f>
+        <v>10196.69</v>
+      </c>
+      <c r="G944" s="10">
+        <f t="shared" si="2"/>
+        <v>12596.98</v>
+      </c>
+      <c r="H944" s="11">
+        <f t="shared" ref="H944:H945" si="3">E944-F944</f>
+        <v>12596.98</v>
+      </c>
+      <c r="I944" s="12">
+        <f>COUNTA(I2:I942)</f>
+        <v>941</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="E945" s="10">
+        <f>E944/I944</f>
+        <v>24.22281615</v>
+      </c>
+      <c r="F945" s="10">
+        <f>F944/I944</f>
+        <v>10.83601488</v>
+      </c>
+      <c r="G945" s="10">
+        <f>G944/I944</f>
+        <v>13.38680128</v>
+      </c>
+      <c r="H945" s="11">
+        <f t="shared" si="3"/>
+        <v>13.38680128</v>
+      </c>
+      <c r="I945" s="12">
+        <f>I944/I944</f>
         <v>1</v>
       </c>
     </row>
-    <row r="943">
-      <c r="G943" s="10"/>
-    </row>
-    <row r="945">
-      <c r="G945" s="10"/>
+    <row r="946">
+      <c r="E946" s="10">
+        <f t="shared" ref="E946:F946" si="4">E944/16</f>
+        <v>1424.604375</v>
+      </c>
+      <c r="F946" s="10">
+        <f t="shared" si="4"/>
+        <v>637.293125</v>
+      </c>
+      <c r="G946" s="10">
+        <f>E946-F946</f>
+        <v>787.31125</v>
+      </c>
+      <c r="I946" s="13" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="G947" s="14"/>
+    </row>
+    <row r="949">
+      <c r="F949" s="12"/>
+      <c r="G949" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$I$938"/>
+  <autoFilter ref="$A$1:$I$942"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H695"/>
     <hyperlink r:id="rId2" ref="H897"/>

</xml_diff>